<commit_message>
Changes to excel files from flat data class
</commit_message>
<xml_diff>
--- a/lessons/free_tidy.xlsx
+++ b/lessons/free_tidy.xlsx
@@ -382,7 +382,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Alabama ....................</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -400,7 +400,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Alaska ..................</t>
+          <t>Alaska</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -418,7 +418,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Arizona .....................</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -436,7 +436,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Arkansas ..................</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -454,7 +454,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>California .................</t>
+          <t>California</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -472,7 +472,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Colorado ....................</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -490,7 +490,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Connecticut ...............</t>
+          <t>Connecticut</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Delaware ..................</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -526,7 +526,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>District of Columbia ........</t>
+          <t>District of Columbia</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Florida ..................</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -562,7 +562,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Georgia ............................</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hawaii .....................</t>
+          <t>Hawaii</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -598,7 +598,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Idaho ........................</t>
+          <t>Idaho</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -616,7 +616,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Illinois .................</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Indiana ....................</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Iowa ........................</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -670,7 +670,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Kansas .....................</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -688,7 +688,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Kentucky .................</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -706,7 +706,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Louisiana ...................</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Maine .....................</t>
+          <t>Maine</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -742,7 +742,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Maryland ....................</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -760,7 +760,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Massachusetts ..............</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -778,7 +778,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Michigan .....................</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -796,7 +796,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Minnesota ...................</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -814,7 +814,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Mississippi .............</t>
+          <t>Mississippi</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -832,7 +832,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Missouri ..................</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -850,7 +850,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Montana .....................</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -868,7 +868,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Nebraska ....................</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -886,7 +886,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Nevada ....................</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -904,7 +904,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>New Hampshire ..................</t>
+          <t>New Hampshire</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -922,7 +922,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>New Jersey .................</t>
+          <t>New Jersey</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -940,7 +940,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>New Mexico .................</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>New York ................</t>
+          <t>New York</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -976,7 +976,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>North Carolina ...........</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -994,7 +994,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>North Dakota ................</t>
+          <t>North Dakota</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1012,7 +1012,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Ohio .......................</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1030,7 +1030,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Oklahoma ....................</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1048,7 +1048,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Oregon ......................</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Pennsylvania ...............</t>
+          <t>Pennsylvania</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1084,7 +1084,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Rhode Island ..............</t>
+          <t>Rhode Island</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1102,7 +1102,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>South Carolina .............</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1120,7 +1120,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>South Dakota .............</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1138,7 +1138,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Tennessee ...............</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1156,7 +1156,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Texas ....................</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1174,7 +1174,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Utah ....................</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1192,7 +1192,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Vermont ....................</t>
+          <t>Vermont</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1210,7 +1210,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Virginia ....................</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1228,7 +1228,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Washington ..................</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1246,7 +1246,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>West Virginia ...........</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1264,7 +1264,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Wisconsin ................</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1282,7 +1282,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Wyoming ...................</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1300,7 +1300,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Alabama ....................</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1318,7 +1318,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Alaska ..................</t>
+          <t>Alaska</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1336,7 +1336,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Arizona .....................</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1354,7 +1354,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Arkansas ..................</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1372,7 +1372,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>California .................</t>
+          <t>California</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1390,7 +1390,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Colorado ....................</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1408,7 +1408,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Connecticut ...............</t>
+          <t>Connecticut</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1426,7 +1426,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Delaware ..................</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1444,7 +1444,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>District of Columbia ........</t>
+          <t>District of Columbia</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1462,7 +1462,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Florida ..................</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1480,7 +1480,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Georgia ............................</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1498,7 +1498,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Hawaii .....................</t>
+          <t>Hawaii</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1516,7 +1516,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Idaho ........................</t>
+          <t>Idaho</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1534,7 +1534,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Illinois .................</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1552,7 +1552,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Indiana ....................</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1570,7 +1570,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Iowa ........................</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1588,7 +1588,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Kansas .....................</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1606,7 +1606,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Kentucky .................</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1624,7 +1624,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Louisiana ...................</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1642,7 +1642,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Maine .....................</t>
+          <t>Maine</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1660,7 +1660,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Maryland ....................</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1678,7 +1678,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Massachusetts ..............</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1696,7 +1696,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Michigan .....................</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1714,7 +1714,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Minnesota ...................</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1732,7 +1732,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Mississippi .............</t>
+          <t>Mississippi</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1750,7 +1750,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Missouri ..................</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1768,7 +1768,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Montana .....................</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1786,7 +1786,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Nebraska ....................</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1804,7 +1804,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Nevada ....................</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1822,7 +1822,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>New Hampshire ..................</t>
+          <t>New Hampshire</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1840,7 +1840,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>New Jersey .................</t>
+          <t>New Jersey</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1858,7 +1858,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>New Mexico .................</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1876,7 +1876,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>New York ................</t>
+          <t>New York</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1894,7 +1894,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>North Carolina ...........</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1912,7 +1912,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>North Dakota ................</t>
+          <t>North Dakota</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1930,7 +1930,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Ohio .......................</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1948,7 +1948,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Oklahoma ....................</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1966,7 +1966,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Oregon ......................</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1984,7 +1984,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Pennsylvania ...............</t>
+          <t>Pennsylvania</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2002,7 +2002,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Rhode Island ..............</t>
+          <t>Rhode Island</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2020,7 +2020,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>South Carolina .............</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2038,7 +2038,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>South Dakota .............</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2056,7 +2056,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Tennessee ...............</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2074,7 +2074,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Texas ....................</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2092,7 +2092,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Utah ....................</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2110,7 +2110,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Vermont ....................</t>
+          <t>Vermont</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2128,7 +2128,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Virginia ....................</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2146,7 +2146,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Washington ..................</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2164,7 +2164,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>West Virginia ...........</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2182,7 +2182,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Wisconsin ................</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2200,7 +2200,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Wyoming ...................</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2218,7 +2218,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Alabama ....................</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2236,7 +2236,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Alaska ..................</t>
+          <t>Alaska</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2254,7 +2254,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Arizona .....................</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2272,7 +2272,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Arkansas ..................</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2290,7 +2290,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>California .................</t>
+          <t>California</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2308,7 +2308,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Colorado ....................</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2326,7 +2326,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Connecticut ...............</t>
+          <t>Connecticut</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -2344,7 +2344,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Delaware ..................</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -2362,7 +2362,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>District of Columbia ........</t>
+          <t>District of Columbia</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -2380,7 +2380,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Florida ..................</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -2398,7 +2398,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Georgia ............................</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -2416,7 +2416,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Hawaii .....................</t>
+          <t>Hawaii</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -2434,7 +2434,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Idaho ........................</t>
+          <t>Idaho</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -2452,7 +2452,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Illinois .................</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -2470,7 +2470,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Indiana ....................</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -2488,7 +2488,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Iowa ........................</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -2506,7 +2506,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Kansas .....................</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -2524,7 +2524,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Kentucky .................</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -2542,7 +2542,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Louisiana ...................</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -2560,7 +2560,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Maine .....................</t>
+          <t>Maine</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -2578,7 +2578,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Maryland ....................</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -2596,7 +2596,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Massachusetts ..............</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -2614,7 +2614,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Michigan .....................</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -2632,7 +2632,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Minnesota ...................</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -2650,7 +2650,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Mississippi .............</t>
+          <t>Mississippi</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -2668,7 +2668,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Missouri ..................</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -2686,7 +2686,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Montana .....................</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -2704,7 +2704,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Nebraska ....................</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -2722,7 +2722,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Nevada ....................</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -2740,7 +2740,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>New Hampshire ..................</t>
+          <t>New Hampshire</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -2758,7 +2758,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>New Jersey .................</t>
+          <t>New Jersey</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -2776,7 +2776,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>New Mexico .................</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -2794,7 +2794,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>New York ................</t>
+          <t>New York</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -2812,7 +2812,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>North Carolina ...........</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -2830,7 +2830,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>North Dakota ................</t>
+          <t>North Dakota</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -2848,7 +2848,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Ohio .......................</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -2866,7 +2866,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Oklahoma ....................</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -2884,7 +2884,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Oregon ......................</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -2902,7 +2902,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Pennsylvania ...............</t>
+          <t>Pennsylvania</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -2920,7 +2920,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Rhode Island ..............</t>
+          <t>Rhode Island</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -2938,7 +2938,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>South Carolina .............</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -2956,7 +2956,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>South Dakota .............</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -2974,7 +2974,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Tennessee ...............</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -2992,7 +2992,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Texas ....................</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -3010,7 +3010,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Utah ....................</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -3028,7 +3028,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Vermont ....................</t>
+          <t>Vermont</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -3046,7 +3046,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Virginia ....................</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -3064,7 +3064,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Washington ..................</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -3082,7 +3082,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>West Virginia ...........</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -3100,7 +3100,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Wisconsin ................</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -3118,7 +3118,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Wyoming ...................</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -3136,7 +3136,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Alabama ....................</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -3154,7 +3154,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Alaska ..................</t>
+          <t>Alaska</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -3172,7 +3172,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Arizona .....................</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -3190,7 +3190,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Arkansas ..................</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -3208,7 +3208,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>California .................</t>
+          <t>California</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -3226,7 +3226,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Colorado ....................</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -3244,7 +3244,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Connecticut ...............</t>
+          <t>Connecticut</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -3262,7 +3262,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Delaware ..................</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -3280,7 +3280,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>District of Columbia ........</t>
+          <t>District of Columbia</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -3298,7 +3298,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Florida ..................</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -3316,7 +3316,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Georgia ............................</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -3334,7 +3334,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Hawaii .....................</t>
+          <t>Hawaii</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -3352,7 +3352,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Idaho ........................</t>
+          <t>Idaho</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -3370,7 +3370,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Illinois .................</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -3388,7 +3388,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Indiana ....................</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -3406,7 +3406,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Iowa ........................</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -3424,7 +3424,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Kansas .....................</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -3442,7 +3442,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Kentucky .................</t>
+          <t>Kentucky</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -3460,7 +3460,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Louisiana ...................</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -3478,7 +3478,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Maine .....................</t>
+          <t>Maine</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -3496,7 +3496,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Maryland ....................</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -3514,7 +3514,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Massachusetts ..............</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -3532,7 +3532,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Michigan .....................</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -3550,7 +3550,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Minnesota ...................</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -3568,7 +3568,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Mississippi .............</t>
+          <t>Mississippi</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -3586,7 +3586,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Missouri ..................</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -3604,7 +3604,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Montana .....................</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -3622,7 +3622,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Nebraska ....................</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -3640,7 +3640,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Nevada ....................</t>
+          <t>Nevada</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -3658,7 +3658,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>New Hampshire ..................</t>
+          <t>New Hampshire</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -3676,7 +3676,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>New Jersey .................</t>
+          <t>New Jersey</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -3694,7 +3694,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>New Mexico .................</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -3712,7 +3712,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>New York ................</t>
+          <t>New York</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -3730,7 +3730,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>North Carolina ...........</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -3748,7 +3748,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>North Dakota ................</t>
+          <t>North Dakota</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -3766,7 +3766,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Ohio .......................</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -3784,7 +3784,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Oklahoma ....................</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -3802,7 +3802,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Oregon ......................</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -3820,7 +3820,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Pennsylvania ...............</t>
+          <t>Pennsylvania</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -3838,7 +3838,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Rhode Island ..............</t>
+          <t>Rhode Island</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -3856,7 +3856,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>South Carolina .............</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -3874,7 +3874,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>South Dakota .............</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -3892,7 +3892,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Tennessee ...............</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Texas ....................</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -3928,7 +3928,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Utah ....................</t>
+          <t>Utah</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -3946,7 +3946,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Vermont ....................</t>
+          <t>Vermont</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -3964,7 +3964,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Virginia ....................</t>
+          <t>Virginia</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -3982,7 +3982,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Washington ..................</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -4000,7 +4000,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>West Virginia ...........</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -4018,7 +4018,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Wisconsin ................</t>
+          <t>Wisconsin</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -4036,7 +4036,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Wyoming ...................</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">

</xml_diff>